<commit_message>
feat:done report 12 and 13
</commit_message>
<xml_diff>
--- a/public/assets/report/report-13.xlsx
+++ b/public/assets/report/report-13.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nuraeni\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\sistem-pelaporan-terpadu-puskesmas\public\assets\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF04050-438B-4612-AD29-7EC2E8A30E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7E1D13-AE29-4256-ACA2-3167FAB52F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <t>Fraktur mahkota yang tidak merusak pulpa</t>
   </si>
   <si>
-    <t>S02.5</t>
-  </si>
-  <si>
     <t>Mengetahui,</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>R51</t>
+  </si>
+  <si>
+    <t>S02.6</t>
   </si>
 </sst>
 </file>
@@ -422,15 +422,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -441,6 +432,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:S1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="50" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="50" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -671,57 +671,57 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="15.6">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
     </row>
     <row r="3" spans="1:19" ht="15.6">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
     </row>
     <row r="5" spans="1:19" ht="24.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -768,19 +768,19 @@
     </row>
     <row r="7" spans="1:19" ht="30.75" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="23"/>
+      <c r="D7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26"/>
       <c r="K7" s="3"/>
       <c r="L7" s="4" t="s">
         <v>8</v>
@@ -798,40 +798,40 @@
       <c r="S7" s="5"/>
     </row>
     <row r="9" spans="1:19" ht="14.4">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="22" t="s">
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="R9" s="23"/>
-      <c r="S9" s="24"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="26"/>
     </row>
     <row r="10" spans="1:19" ht="26.4">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="8" t="s">
         <v>15</v>
       </c>
@@ -1022,40 +1022,40 @@
       <c r="S14" s="13"/>
     </row>
     <row r="16" spans="1:19" ht="14.4">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="22" t="s">
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="R16" s="23"/>
-      <c r="S16" s="24"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:19" ht="26.4">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
@@ -1382,40 +1382,40 @@
     </row>
     <row r="27" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="22" t="s">
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="R28" s="23"/>
-      <c r="S28" s="24"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="8" t="s">
         <v>15</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>50</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -1559,7 +1559,7 @@
         <v>51</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
@@ -1582,16 +1582,16 @@
     <row r="34" spans="1:15" ht="15.75" customHeight="1"/>
     <row r="35" spans="1:15" ht="15.75" customHeight="1">
       <c r="A35" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O35" s="17"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1">
       <c r="A36" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="O36" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1">
@@ -1605,22 +1605,22 @@
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="O40" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="O41" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1"/>
@@ -2585,11 +2585,6 @@
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A2:S2"/>
-    <mergeCell ref="A3:S3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:J7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="Q9:S9"/>
@@ -2605,6 +2600,11 @@
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:P16"/>
     <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="70" orientation="landscape"/>

</xml_diff>